<commit_message>
se agrego costo de disenio a interfaz de Pedido
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>Indice</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>En el pedido de operador, siempre mostrar los kg, pero que tambien se puedan registrar pz</t>
+  </si>
+  <si>
+    <t>Agregar JoptionPane en todos los botones</t>
+  </si>
+  <si>
+    <t>Se agrego al interfaz</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:C31"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,6 +942,34 @@
       </c>
       <c r="C31" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7.1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>43798</v>
+      </c>
+      <c r="E33" s="1">
+        <v>43798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se integraron todos los cambios necesarios en Pedido para que el costo de diseño no tenga errores
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\sistema-imprexa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D54A69-18C9-4165-8589-5E03F4407F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D20D2-3741-4870-B2F4-6100F9081304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>Indice</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>detalles partida siempre selecciona pz finales al abrirlo</t>
+  </si>
+  <si>
+    <t>se creo el campo costoDisenio en la base</t>
+  </si>
+  <si>
+    <t>se deshabilito para guardar datos en procesos</t>
+  </si>
+  <si>
+    <t>se hace el guardado y se integro de pedido</t>
+  </si>
+  <si>
+    <t>preguntar si afectara a la formula de pyg</t>
+  </si>
+  <si>
+    <t>añadirlo a la tabla de pedido de visualizacion y quitarlo de la de produccion</t>
+  </si>
+  <si>
+    <t>añadirlo a detallesPedido</t>
   </si>
 </sst>
 </file>
@@ -210,10 +228,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15E5CD8D-9415-4893-B6A2-533381395684}" name="Tabla2" displayName="Tabla2" ref="A1:E38" totalsRowShown="0">
-  <autoFilter ref="A1:E38" xr:uid="{055744EF-73B6-49FD-843F-728F1456344D}"/>
-  <sortState ref="A2:E38">
-    <sortCondition ref="A1:A38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15E5CD8D-9415-4893-B6A2-533381395684}" name="Tabla2" displayName="Tabla2" ref="A1:E44" totalsRowShown="0">
+  <autoFilter ref="A1:E44" xr:uid="{055744EF-73B6-49FD-843F-728F1456344D}"/>
+  <sortState ref="A2:E44">
+    <sortCondition ref="A1:A44"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DBE4A8BE-223D-4DA7-8B8A-83EC6C4C599C}" name="Indice"/>
@@ -547,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,7 +997,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>7.1</v>
+        <v>7.01</v>
       </c>
       <c r="B28" t="s">
         <v>38</v>
@@ -996,43 +1014,61 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>8</v>
+        <v>7.02</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>43803</v>
+      </c>
+      <c r="E29" s="1">
+        <v>43803</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>9</v>
+        <v>7.03</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>43803</v>
+      </c>
+      <c r="E30" s="1">
+        <v>43803</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>10</v>
+        <v>7.04</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D31" s="1">
+        <v>43803</v>
+      </c>
+      <c r="E31" s="1">
+        <v>43803</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>11</v>
+        <v>7.05</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -1040,10 +1076,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>12</v>
+        <v>7.06</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -1051,10 +1087,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>13</v>
+        <v>7.07</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -1062,10 +1098,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1073,10 +1109,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -1084,10 +1120,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
@@ -1095,19 +1131,86 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>17</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
se agrego la columna diseño a la tabla de pedido en Visualizacion
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\sistema-imprexa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06F3DEA-3EB8-42D2-861E-769855CFDC8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D90E332-0010-4374-B9E9-74C0DFD2A18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D33" sqref="D33:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.06</v>
       </c>
@@ -1082,10 +1082,16 @@
         <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>43803</v>
+      </c>
+      <c r="E33" s="1">
+        <v>43803</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.07</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>11</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12</v>
       </c>
@@ -1151,7 +1157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>13</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1173,7 +1179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>15</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>16</v>
       </c>
@@ -1195,7 +1201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
se añadio estatus a Pedido y a la base de datos
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\sistema-imprexa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D90E332-0010-4374-B9E9-74C0DFD2A18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816B14A-0369-4201-A87F-D0966EEC3897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>Indice</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Agregar costo de diseño a pedido</t>
   </si>
   <si>
-    <t>Agregar estatus a la visualizacion, al lado de fecha de ingreso</t>
-  </si>
-  <si>
     <t>Ajustar tablas de visualizacion, en partidas, maximo 4</t>
   </si>
   <si>
@@ -172,6 +169,30 @@
   </si>
   <si>
     <t>añadirlo a detallesPedido</t>
+  </si>
+  <si>
+    <t>cambiar el formato de la fecha que se muestra en el reporte de produccion</t>
+  </si>
+  <si>
+    <t>agregarlo a la interfaz</t>
+  </si>
+  <si>
+    <t>agregarlo a la base de datos</t>
+  </si>
+  <si>
+    <t>que se pueda guardar</t>
+  </si>
+  <si>
+    <t>integrarlo a todas las funcionalidades de Pedido</t>
+  </si>
+  <si>
+    <t>que se muestre en la visualizacion, a un lado de la fecha de ingreso</t>
+  </si>
+  <si>
+    <t>que se pueda modificar en detalles pedido</t>
+  </si>
+  <si>
+    <t>quitarlo de partidas</t>
   </si>
 </sst>
 </file>
@@ -228,10 +249,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15E5CD8D-9415-4893-B6A2-533381395684}" name="Tabla2" displayName="Tabla2" ref="A1:E44" totalsRowShown="0">
-  <autoFilter ref="A1:E44" xr:uid="{055744EF-73B6-49FD-843F-728F1456344D}"/>
-  <sortState ref="A2:E44">
-    <sortCondition ref="A1:A44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15E5CD8D-9415-4893-B6A2-533381395684}" name="Tabla2" displayName="Tabla2" ref="A1:E51" totalsRowShown="0">
+  <autoFilter ref="A1:E51" xr:uid="{055744EF-73B6-49FD-843F-728F1456344D}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="no"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A25:E51">
+    <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DBE4A8BE-223D-4DA7-8B8A-83EC6C4C599C}" name="Indice"/>
@@ -565,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -606,7 +633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -617,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -628,7 +655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.1</v>
       </c>
@@ -645,7 +672,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3.2</v>
       </c>
@@ -662,7 +689,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.3</v>
       </c>
@@ -679,7 +706,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.4</v>
       </c>
@@ -696,7 +723,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -707,7 +734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4.01</v>
       </c>
@@ -724,7 +751,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0199999999999996</v>
       </c>
@@ -741,7 +768,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4.03</v>
       </c>
@@ -758,7 +785,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4.04</v>
       </c>
@@ -775,7 +802,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4.05</v>
       </c>
@@ -792,7 +819,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4.0599999999999996</v>
       </c>
@@ -809,7 +836,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4.07</v>
       </c>
@@ -826,7 +853,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4.08</v>
       </c>
@@ -843,7 +870,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4.09</v>
       </c>
@@ -860,7 +887,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4.0999999999999996</v>
       </c>
@@ -877,7 +904,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4.12</v>
       </c>
@@ -894,7 +921,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4.13</v>
       </c>
@@ -911,7 +938,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4.1399999999999997</v>
       </c>
@@ -928,7 +955,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4.1500000000000004</v>
       </c>
@@ -945,7 +972,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4.16</v>
       </c>
@@ -973,7 +1000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -995,12 +1022,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7.01</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1012,12 +1039,12 @@
         <v>43798</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7.02</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -1029,12 +1056,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7.03</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -1046,12 +1073,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7.04</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -1068,18 +1095,18 @@
         <v>7.05</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.06</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1091,15 +1118,21 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.07</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D34" s="1">
+        <v>43803</v>
+      </c>
+      <c r="E34" s="1">
+        <v>43803</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1115,32 +1148,32 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9</v>
+        <v>8.01</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>10</v>
+        <v>8.02</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>11</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
@@ -1148,10 +1181,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>12</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -1159,10 +1192,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>13</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
@@ -1170,10 +1203,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>14</v>
+        <v>8.06</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
@@ -1181,10 +1214,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
@@ -1192,10 +1225,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -1203,12 +1236,89 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>17</v>
       </c>
-      <c r="B44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>8.07</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se hizo en imprexa, se permite visualizar al segundo preoveedor de impreso en Visualizacion, se añadieron mas tareas
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E0671A-3C46-4750-997F-8549B7CAA401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>Indice</t>
   </si>
@@ -193,12 +187,27 @@
   </si>
   <si>
     <t>detalles partida siempre selecciona pz finales al abrirlo, y no cambia de checkbox al pasar entre partidas</t>
+  </si>
+  <si>
+    <t>Acomodar todos los rs y st</t>
+  </si>
+  <si>
+    <t>si el pedido ya se pago, que se muestre 0 en resto</t>
+  </si>
+  <si>
+    <t>Preguntar que hacer con sticky</t>
+  </si>
+  <si>
+    <t>copia en dos pc</t>
+  </si>
+  <si>
+    <t>copia en la nube</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,10 +244,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,8 +267,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15E5CD8D-9415-4893-B6A2-533381395684}" name="Tabla2" displayName="Tabla2" ref="A1:E51" totalsRowShown="0">
-  <autoFilter ref="A1:E51" xr:uid="{055744EF-73B6-49FD-843F-728F1456344D}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E56" totalsRowShown="0">
+  <autoFilter ref="A1:E56">
     <filterColumn colId="2">
       <filters>
         <filter val="no"/>
@@ -269,11 +279,11 @@
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DBE4A8BE-223D-4DA7-8B8A-83EC6C4C599C}" name="Indice"/>
-    <tableColumn id="2" xr3:uid="{6582F038-4BDF-4706-980E-085B6D1C53BB}" name="Descripción"/>
-    <tableColumn id="3" xr3:uid="{592E3675-3DAA-4D4C-8891-9E80B66D1E76}" name="Terminado"/>
-    <tableColumn id="4" xr3:uid="{1DB3EA8D-C6C7-44C5-AFD8-82C07FE5D77C}" name="Fecha inicio"/>
-    <tableColumn id="5" xr3:uid="{6DD71490-1D64-4791-BFD1-FB10FA9C55F6}" name="Fecha fin"/>
+    <tableColumn id="1" name="Indice"/>
+    <tableColumn id="2" name="Descripción"/>
+    <tableColumn id="3" name="Terminado"/>
+    <tableColumn id="4" name="Fecha inicio"/>
+    <tableColumn id="5" name="Fecha fin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -322,7 +332,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,26 +365,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,23 +400,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -599,11 +575,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +973,7 @@
         <v>43797</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1005,7 +981,13 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43805</v>
+      </c>
+      <c r="E25" s="1">
+        <v>43805</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1102,7 +1084,7 @@
       <c r="A32">
         <v>7.05</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C32" t="s">
@@ -1143,7 +1125,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1151,7 +1133,13 @@
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D35" s="1">
+        <v>43804</v>
+      </c>
+      <c r="E35" s="1">
+        <v>43804</v>
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1260,7 +1248,7 @@
       <c r="A42">
         <v>8.07</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C42" t="s">
@@ -1282,7 +1270,7 @@
       <c r="A44">
         <v>11</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C44" t="s">
@@ -1319,6 +1307,9 @@
       <c r="D46" s="1">
         <v>43804</v>
       </c>
+      <c r="E46" s="1">
+        <v>43804</v>
+      </c>
     </row>
     <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -1346,7 +1337,7 @@
       <c r="A49">
         <v>16</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C49" t="s">
@@ -1372,6 +1363,61 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>19</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>21</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>22</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>23</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1385,7 +1431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1397,7 +1443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
se añadieron nuevas tareas
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
   <si>
     <t>Indice</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>copia en la nube</t>
+  </si>
+  <si>
+    <t>Al ultimo comboBox de tintas se le agregaran las tintas especiales que me dara reme</t>
+  </si>
+  <si>
+    <t>multiplicar los cm2 de sticky por el precio(foto) y restarlo a las ganancias</t>
   </si>
 </sst>
 </file>
@@ -267,8 +273,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E56" totalsRowShown="0">
-  <autoFilter ref="A1:E56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E58" totalsRowShown="0">
+  <autoFilter ref="A1:E58">
     <filterColumn colId="2">
       <filters>
         <filter val="no"/>
@@ -576,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,7 +1387,7 @@
       <c r="A53">
         <v>20</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C53" t="s">
@@ -1419,6 +1425,22 @@
       </c>
       <c r="C56" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>16.010000000000002</v>
+      </c>
+      <c r="B57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>21.01</v>
+      </c>
+      <c r="B58" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregaron nuevas tareas
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AF4E68-DDFF-4287-A272-5C22F79851F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="82">
   <si>
     <t>Indice</t>
   </si>
@@ -237,9 +231,6 @@
     <t>permitir cambiar sticky desde detallesPedido</t>
   </si>
   <si>
-    <t>Mejorar el acomodo en la tabla de pedido de Visualizacion</t>
-  </si>
-  <si>
     <t>mostrar los nuevos datos de procesos en visualizacion</t>
   </si>
   <si>
@@ -258,19 +249,25 @@
     <t>checar que restaure desde el servidor</t>
   </si>
   <si>
-    <t>checar que haga la restauracion desde el usuario</t>
-  </si>
-  <si>
-    <t>checar que haga la copia en el usuario</t>
-  </si>
-  <si>
     <t>Agregar loggins donde hay printstacktrace</t>
+  </si>
+  <si>
+    <t>investigar como guardar copia en servidor desde usuario</t>
+  </si>
+  <si>
+    <t>investigar como restaurar copia en servidor desde usuario</t>
+  </si>
+  <si>
+    <t>Mejorar el acomodo del interfaz</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,11 +327,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
-  <autoFilter ref="A1:E75" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E74" totalsRowShown="0">
+  <autoFilter ref="A1:E74">
     <filterColumn colId="2">
-      <filters>
+      <filters blank="1">
         <filter val="en espera"/>
+        <filter val="En proceso"/>
         <filter val="no"/>
       </filters>
     </filterColumn>
@@ -343,11 +341,11 @@
     <sortCondition ref="A1:A74"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Indice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Terminado"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha inicio"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fecha fin"/>
+    <tableColumn id="1" name="Indice"/>
+    <tableColumn id="2" name="Descripción"/>
+    <tableColumn id="3" name="Terminado"/>
+    <tableColumn id="4" name="Fecha inicio"/>
+    <tableColumn id="5" name="Fecha fin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -396,7 +394,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -429,26 +427,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,23 +462,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -673,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1150,7 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1468,89 +1432,105 @@
         <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1">
+        <v>43810</v>
+      </c>
+      <c r="E51" s="1">
+        <v>43810</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="1">
-        <v>43810</v>
-      </c>
-      <c r="E52" s="1">
-        <v>43810</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>19</v>
-      </c>
-      <c r="B53" t="s">
-        <v>56</v>
+        <v>20</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D53" s="1">
+        <v>43809</v>
+      </c>
+      <c r="E53" s="1">
+        <v>43809</v>
       </c>
     </row>
     <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
-      </c>
-      <c r="D54" s="1">
-        <v>43809</v>
-      </c>
-      <c r="E54" s="1">
-        <v>43809</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>21</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>58</v>
+        <v>21.01</v>
+      </c>
+      <c r="B55" t="s">
+        <v>62</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
+      </c>
+      <c r="D55" s="1">
+        <v>43805</v>
+      </c>
+      <c r="E55" s="1">
+        <v>43805</v>
       </c>
     </row>
     <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>21.01</v>
+        <v>21.02</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1">
-        <v>43805</v>
+        <v>43808</v>
       </c>
       <c r="E56" s="1">
-        <v>43805</v>
+        <v>43808</v>
       </c>
     </row>
     <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>21.02</v>
+        <v>21.03</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1564,10 +1544,10 @@
     </row>
     <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>21.03</v>
+        <v>21.04</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1581,10 +1561,10 @@
     </row>
     <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>21.04</v>
+        <v>21.05</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1598,10 +1578,10 @@
     </row>
     <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>21.05</v>
+        <v>21.06</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1615,10 +1595,10 @@
     </row>
     <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>21.06</v>
+        <v>21.07</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1632,10 +1612,10 @@
     </row>
     <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>21.07</v>
+        <v>21.08</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1647,76 +1627,76 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>21.08</v>
-      </c>
-      <c r="B63" t="s">
-        <v>70</v>
+        <v>22</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="1">
-        <v>43808</v>
-      </c>
-      <c r="E63" s="1">
-        <v>43808</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>22</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>59</v>
+        <v>22.03</v>
+      </c>
+      <c r="B64" t="s">
+        <v>78</v>
       </c>
       <c r="C64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>24</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="1">
+        <v>43810</v>
+      </c>
+      <c r="E65" s="1">
+        <v>43810</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>22.04</v>
+      </c>
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>22.03</v>
-      </c>
-      <c r="B65" t="s">
-        <v>79</v>
-      </c>
-      <c r="C65" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>24</v>
-      </c>
-      <c r="B66" t="s">
-        <v>67</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="1">
-        <v>43810</v>
-      </c>
-      <c r="E66" s="1">
-        <v>43810</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>22.04</v>
+        <v>26</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D67" s="1">
+        <v>43811</v>
+      </c>
+      <c r="E67" s="1">
+        <v>43811</v>
       </c>
     </row>
     <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>26</v>
+        <v>26.01</v>
       </c>
       <c r="B68" t="s">
         <v>72</v>
@@ -1733,7 +1713,7 @@
     </row>
     <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>26.01</v>
+        <v>26.02</v>
       </c>
       <c r="B69" t="s">
         <v>73</v>
@@ -1750,24 +1730,18 @@
     </row>
     <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>26.02</v>
+        <v>22.01</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
-      </c>
-      <c r="D70" s="1">
-        <v>43811</v>
-      </c>
-      <c r="E70" s="1">
-        <v>43811</v>
       </c>
     </row>
     <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>22.01</v>
+        <v>22.02</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
@@ -1776,23 +1750,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>22.02</v>
+        <v>23</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C72" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>23</v>
-      </c>
-      <c r="B73" t="s">
-        <v>60</v>
+        <v>25</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C73" t="s">
         <v>11</v>
@@ -1800,23 +1774,12 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>25</v>
-      </c>
-      <c r="B74" t="s">
-        <v>71</v>
+        <v>26</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>26</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C75" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1830,7 +1793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1842,7 +1805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
se modificaron las tareas
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -641,7 +641,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1674,7 @@
         <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
hubo un problema al pushear, este commit reune 4 commits. que se encargaron de acomodar el codigo de procesos, crear una clase solo para la documentacion y permitir la restauracion desde el servidor o el cliente
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8EF18F-A1EF-44D5-A2DF-381EB1B99A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -267,7 +273,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -327,10 +333,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E74" totalsRowShown="0">
-  <autoFilter ref="A1:E74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:E74" totalsRowShown="0">
+  <autoFilter ref="A1:E74" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="2">
-      <filters blank="1">
+      <filters>
         <filter val="en espera"/>
         <filter val="En proceso"/>
         <filter val="no"/>
@@ -341,11 +347,11 @@
     <sortCondition ref="A1:A74"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Indice"/>
-    <tableColumn id="2" name="Descripción"/>
-    <tableColumn id="3" name="Terminado"/>
-    <tableColumn id="4" name="Fecha inicio"/>
-    <tableColumn id="5" name="Fecha fin"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Indice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Terminado"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha inicio"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fecha fin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -394,7 +400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,9 +433,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,6 +485,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -637,11 +677,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1667,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>22</v>
       </c>
@@ -1635,10 +1675,10 @@
         <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>22.03</v>
       </c>
@@ -1646,7 +1686,7 @@
         <v>78</v>
       </c>
       <c r="C64" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1666,7 +1706,7 @@
         <v>43810</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>22.04</v>
       </c>
@@ -1674,7 +1714,7 @@
         <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1793,7 +1833,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1805,7 +1845,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
se revisaron los st y rs 2,3,4... hasta la clase GastosFijos
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\sistema-imprexa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8EF18F-A1EF-44D5-A2DF-381EB1B99A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB661C7-A8E6-4526-87CC-4E746085C485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
   <si>
     <t>Indice</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>En proceso</t>
+  </si>
+  <si>
+    <t>Cambiar los loggin por printstacktrace</t>
   </si>
 </sst>
 </file>
@@ -333,8 +336,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:E74" totalsRowShown="0">
-  <autoFilter ref="A1:E74" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
+  <autoFilter ref="A1:E75" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="en espera"/>
@@ -678,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,12 +1817,23 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>26</v>
+      </c>
+      <c r="B75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se corrigio hasta Procesos, de Procesos solo los rs y st
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\sistema-imprexa\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB661C7-A8E6-4526-87CC-4E746085C485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -159,9 +153,6 @@
     <t>se hace el guardado y se integro de pedido</t>
   </si>
   <si>
-    <t>preguntar si afectara a la formula de pyg</t>
-  </si>
-  <si>
     <t>añadirlo a la tabla de pedido de visualizacion y quitarlo de la de produccion</t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>copia en dos pc</t>
   </si>
   <si>
-    <t>copia en la nube</t>
-  </si>
-  <si>
     <t>Al ultimo comboBox de tintas se le agregaran las tintas especiales que me dara reme</t>
   </si>
   <si>
@@ -255,9 +243,6 @@
     <t>checar que restaure desde el servidor</t>
   </si>
   <si>
-    <t>Agregar loggins donde hay printstacktrace</t>
-  </si>
-  <si>
     <t>investigar como guardar copia en servidor desde usuario</t>
   </si>
   <si>
@@ -271,12 +256,21 @@
   </si>
   <si>
     <t>Cambiar los loggin por printstacktrace</t>
+  </si>
+  <si>
+    <t>preguntar si afectara a la formula de pyg(ya, no afecta)</t>
+  </si>
+  <si>
+    <t>Agregar JoptionPane a los catch</t>
+  </si>
+  <si>
+    <t>Probar si funciones anidadas mandan muchos errores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,8 +330,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
-  <autoFilter ref="A1:E75" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
+  <autoFilter ref="A1:E75">
     <filterColumn colId="2">
       <filters>
         <filter val="en espera"/>
@@ -350,11 +344,11 @@
     <sortCondition ref="A1:A74"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Indice"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Terminado"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha inicio"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fecha fin"/>
+    <tableColumn id="1" name="Indice"/>
+    <tableColumn id="2" name="Descripción"/>
+    <tableColumn id="3" name="Terminado"/>
+    <tableColumn id="4" name="Fecha inicio"/>
+    <tableColumn id="5" name="Fecha fin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -403,7 +397,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,26 +430,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,23 +465,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -680,11 +640,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1114,7 +1074,7 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1185,15 +1145,15 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7.05</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>45</v>
+      <c r="B32" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1201,7 +1161,7 @@
         <v>7.06</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1218,7 +1178,7 @@
         <v>7.07</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1252,7 +1212,7 @@
         <v>8.01</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1269,7 +1229,7 @@
         <v>8.02</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1286,7 +1246,7 @@
         <v>8.0299999999999994</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1303,7 +1263,7 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1320,7 +1280,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1337,7 +1297,7 @@
         <v>8.06</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1354,7 +1314,7 @@
         <v>8.07</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1472,10 +1432,10 @@
         <v>16.010000000000002</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1483,7 +1443,7 @@
         <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1500,10 +1460,10 @@
         <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1511,7 +1471,7 @@
         <v>20</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1528,7 +1488,7 @@
         <v>21</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1539,7 +1499,7 @@
         <v>21.01</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1556,7 +1516,7 @@
         <v>21.02</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1573,7 +1533,7 @@
         <v>21.03</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1590,7 +1550,7 @@
         <v>21.04</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1607,7 +1567,7 @@
         <v>21.05</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1624,7 +1584,7 @@
         <v>21.06</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1641,7 +1601,7 @@
         <v>21.07</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1658,7 +1618,7 @@
         <v>21.08</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1675,7 +1635,7 @@
         <v>22</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -1686,7 +1646,7 @@
         <v>22.03</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1697,7 +1657,7 @@
         <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -1714,7 +1674,7 @@
         <v>22.04</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -1725,7 +1685,7 @@
         <v>26</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -1742,7 +1702,7 @@
         <v>26.01</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -1759,7 +1719,7 @@
         <v>26.02</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -1776,7 +1736,7 @@
         <v>22.01</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -1787,7 +1747,7 @@
         <v>22.02</v>
       </c>
       <c r="B71" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -1795,10 +1755,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>23</v>
-      </c>
-      <c r="B72" t="s">
-        <v>60</v>
+        <v>25</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C72" t="s">
         <v>11</v>
@@ -1806,10 +1766,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>25</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>80</v>
+        <v>26</v>
+      </c>
+      <c r="B73" t="s">
+        <v>79</v>
       </c>
       <c r="C73" t="s">
         <v>11</v>
@@ -1817,10 +1777,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>27</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>77</v>
+        <v>26.02</v>
+      </c>
+      <c r="B74" t="s">
+        <v>81</v>
       </c>
       <c r="C74" t="s">
         <v>11</v>
@@ -1828,7 +1788,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>26</v>
+        <v>26.01</v>
       </c>
       <c r="B75" t="s">
         <v>82</v>
@@ -1847,7 +1807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1859,7 +1819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
se cambiaron todos los logger por printStackTrace
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\sistema-imprexa\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3BD3F2-4865-4C0E-A439-0BD3974F7CEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
   <si>
     <t>Indice</t>
   </si>
@@ -250,9 +256,6 @@
   </si>
   <si>
     <t>Mejorar el acomodo del interfaz</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
   <si>
     <t>Cambiar los loggin por printstacktrace</t>
@@ -270,18 +273,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,10 +303,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -330,25 +325,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
-  <autoFilter ref="A1:E75">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="en espera"/>
-        <filter val="En proceso"/>
-        <filter val="no"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A27:E74">
-    <sortCondition ref="A1:A74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
+  <autoFilter ref="A1:E75" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState ref="A2:E75">
+    <sortCondition ref="A1:A75"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Indice"/>
-    <tableColumn id="2" name="Descripción"/>
-    <tableColumn id="3" name="Terminado"/>
-    <tableColumn id="4" name="Fecha inicio"/>
-    <tableColumn id="5" name="Fecha fin"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Indice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Terminado"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha inicio"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fecha fin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -397,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,9 +417,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,6 +469,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -640,11 +661,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -682,7 +703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -693,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -704,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.1</v>
       </c>
@@ -721,7 +742,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3.2</v>
       </c>
@@ -738,7 +759,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.3</v>
       </c>
@@ -755,7 +776,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.4</v>
       </c>
@@ -772,7 +793,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -783,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4.01</v>
       </c>
@@ -800,7 +821,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0199999999999996</v>
       </c>
@@ -817,7 +838,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4.03</v>
       </c>
@@ -834,7 +855,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4.04</v>
       </c>
@@ -851,7 +872,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4.05</v>
       </c>
@@ -868,7 +889,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4.0599999999999996</v>
       </c>
@@ -885,7 +906,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4.07</v>
       </c>
@@ -902,7 +923,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4.08</v>
       </c>
@@ -919,7 +940,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4.09</v>
       </c>
@@ -936,7 +957,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4.0999999999999996</v>
       </c>
@@ -953,7 +974,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4.12</v>
       </c>
@@ -970,7 +991,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4.13</v>
       </c>
@@ -987,7 +1008,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4.1399999999999997</v>
       </c>
@@ -1004,7 +1025,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4.1500000000000004</v>
       </c>
@@ -1021,7 +1042,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4.16</v>
       </c>
@@ -1038,7 +1059,7 @@
         <v>43797</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1055,7 +1076,7 @@
         <v>43805</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1066,7 +1087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1077,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7.01</v>
       </c>
@@ -1094,7 +1115,7 @@
         <v>43798</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7.02</v>
       </c>
@@ -1111,7 +1132,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7.03</v>
       </c>
@@ -1128,7 +1149,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7.04</v>
       </c>
@@ -1145,18 +1166,18 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7.05</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>80</v>
+      <c r="B32" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.06</v>
       </c>
@@ -1173,7 +1194,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.07</v>
       </c>
@@ -1190,7 +1211,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1207,7 +1228,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8.01</v>
       </c>
@@ -1224,7 +1245,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8.02</v>
       </c>
@@ -1241,7 +1262,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>8.0299999999999994</v>
       </c>
@@ -1258,7 +1279,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8.0399999999999991</v>
       </c>
@@ -1275,7 +1296,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8.0500000000000007</v>
       </c>
@@ -1292,7 +1313,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8.06</v>
       </c>
@@ -1309,18 +1330,18 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>8.07</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>10</v>
       </c>
@@ -1337,11 +1358,11 @@
         <v>43809</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>11</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C44" t="s">
@@ -1354,7 +1375,7 @@
         <v>42709</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>12</v>
       </c>
@@ -1371,7 +1392,7 @@
         <v>43810</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>13</v>
       </c>
@@ -1388,7 +1409,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14</v>
       </c>
@@ -1399,7 +1420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>15</v>
       </c>
@@ -1420,7 +1441,7 @@
       <c r="A49">
         <v>16</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C49" t="s">
@@ -1438,11 +1459,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>18</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C51" t="s">
@@ -1459,14 +1480,14 @@
       <c r="A52">
         <v>19</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>20</v>
       </c>
@@ -1483,7 +1504,7 @@
         <v>43809</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>21</v>
       </c>
@@ -1494,11 +1515,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>21.01</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C55" t="s">
@@ -1511,11 +1532,11 @@
         <v>43805</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>21.02</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C56" t="s">
@@ -1528,7 +1549,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21.03</v>
       </c>
@@ -1545,7 +1566,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>21.04</v>
       </c>
@@ -1562,7 +1583,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>21.05</v>
       </c>
@@ -1579,7 +1600,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>21.06</v>
       </c>
@@ -1596,7 +1617,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>21.07</v>
       </c>
@@ -1613,7 +1634,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>21.08</v>
       </c>
@@ -1630,7 +1651,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>22</v>
       </c>
@@ -1641,138 +1662,132 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
+        <v>22.01</v>
+      </c>
+      <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>22.02</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>22.03</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>75</v>
       </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>22.04</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>24</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" t="s">
         <v>65</v>
       </c>
-      <c r="C65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="1">
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="1">
         <v>43810</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E68" s="1">
         <v>43810</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>22.04</v>
-      </c>
-      <c r="B66" t="s">
-        <v>76</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>25</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>26</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B70" t="s">
         <v>69</v>
       </c>
-      <c r="C67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="1">
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="1">
         <v>43811</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E70" s="1">
         <v>43811</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>26.01</v>
-      </c>
-      <c r="B68" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="1">
-        <v>43811</v>
-      </c>
-      <c r="E68" s="1">
-        <v>43811</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>26.02</v>
-      </c>
-      <c r="B69" t="s">
-        <v>71</v>
-      </c>
-      <c r="C69" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="1">
-        <v>43811</v>
-      </c>
-      <c r="E69" s="1">
-        <v>43811</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>22.01</v>
-      </c>
-      <c r="B70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>22.02</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>25</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>77</v>
+        <v>26.01</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D72" s="1">
+        <v>43811</v>
+      </c>
+      <c r="E72" s="1">
+        <v>43811</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>26</v>
+        <v>26.01</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,18 +1795,24 @@
         <v>26.02</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D74" s="1">
+        <v>43811</v>
+      </c>
+      <c r="E74" s="1">
+        <v>43811</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>26.01</v>
+        <v>26.02</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -1807,7 +1828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1819,7 +1840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
se hizo una pequeña correccion en Pedido
</commit_message>
<xml_diff>
--- a/control de progreso.xlsx
+++ b/control de progreso.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\sistema-imprexa\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85574966-4AB6-48CF-9F6C-ECF8E90D6110}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="80">
   <si>
     <t>Indice</t>
   </si>
@@ -49,9 +55,6 @@
   </si>
   <si>
     <t>Agregar donde ver el nuevo proveedor de impreso</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>Revisar formulas relacionadas con IVA y subtotal en todas las clases relacionadas</t>
@@ -264,7 +267,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -316,23 +319,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
-  <autoFilter ref="A1:E75">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="no"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:E75" totalsRowShown="0">
+  <autoFilter ref="A1:E75" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A69:E75">
     <sortCondition ref="C1:C75"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Indice"/>
-    <tableColumn id="2" name="Descripción"/>
-    <tableColumn id="3" name="Terminado"/>
-    <tableColumn id="4" name="Fecha inicio"/>
-    <tableColumn id="5" name="Fecha fin"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Indice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Terminado"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha inicio"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fecha fin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -381,7 +378,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,9 +411,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,6 +463,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -624,11 +655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -666,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -677,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -688,12 +719,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3.1</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -705,12 +736,12 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3.2</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -722,12 +753,12 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.3</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -739,12 +770,12 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.4</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -756,7 +787,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -767,12 +798,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4.01</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -784,12 +815,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0199999999999996</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -801,12 +832,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4.03</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -818,12 +849,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4.04</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -835,12 +866,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4.05</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -852,12 +883,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4.0599999999999996</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -869,12 +900,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4.07</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -886,12 +917,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4.08</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -903,12 +934,12 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4.09</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -920,12 +951,12 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4.0999999999999996</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -937,12 +968,12 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4.12</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -954,12 +985,12 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4.13</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -971,12 +1002,12 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4.1399999999999997</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -988,12 +1019,12 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4.1500000000000004</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -1005,12 +1036,12 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4.16</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1022,7 +1053,7 @@
         <v>43797</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1039,34 +1070,34 @@
         <v>43805</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7.01</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1078,12 +1109,12 @@
         <v>43798</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7.02</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -1095,12 +1126,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7.03</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -1112,12 +1143,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7.04</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -1129,23 +1160,23 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7.05</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.06</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1157,12 +1188,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.07</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1174,12 +1205,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -1191,12 +1222,12 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8.01</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1208,12 +1239,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8.02</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1225,12 +1256,12 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>8.0299999999999994</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1242,12 +1273,12 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8.0399999999999991</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1259,12 +1290,12 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8.0500000000000007</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1276,12 +1307,12 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8.06</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1293,23 +1324,23 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>8.07</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1321,12 +1352,12 @@
         <v>43809</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1338,12 +1369,12 @@
         <v>42709</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1355,12 +1386,12 @@
         <v>43810</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1372,23 +1403,23 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1400,34 +1431,34 @@
         <v>43809</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>16</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>16.010000000000002</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>18</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1439,23 +1470,23 @@
         <v>43810</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>20</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1467,23 +1498,23 @@
         <v>43809</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>21</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>21.01</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1495,12 +1526,12 @@
         <v>43805</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>21.02</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1512,12 +1543,12 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21.03</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1529,12 +1560,12 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>21.04</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1546,12 +1577,12 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>21.05</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1563,12 +1594,12 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>21.06</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1580,12 +1611,12 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>21.07</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1597,12 +1628,12 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>21.08</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1614,67 +1645,67 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>22</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>22.01</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>22.02</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>22.03</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>22.04</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>24</v>
       </c>
       <c r="B68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -1691,18 +1722,18 @@
         <v>25</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -1719,18 +1750,18 @@
         <v>26.02</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>26.01</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -1742,23 +1773,23 @@
         <v>43811</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>26.01</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>26.02</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -1770,12 +1801,12 @@
         <v>43811</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -1794,7 +1825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1806,7 +1837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>